<commit_message>
fixed extra browser opening in each script; added implicit wait
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC349D4-118B-4A5C-84DE-4A43863D88C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743718B4-1B4D-43B4-9BD6-9B4B0806779D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -57,26 +57,6 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Prostate','Bladder, Urethra']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Prostate','Bladder, Urethra']
  WITH DISTINCT samp AS samp, c, demo, diag
@@ -130,6 +110,25 @@
   </si>
   <si>
     <t>TC01_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite_WebData.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Prostate','Bladder, Urethra']
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
+        coalesce(demo.sex, '') AS Sex ,
+        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+        coalesce(demo.weight, '') AS `Weight (kg)`,
+        coalesce(diag.best_response, '') AS `Response to Treatment` </t>
   </si>
 </sst>
 </file>
@@ -501,19 +500,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -530,58 +529,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>